<commit_message>
Add plein de choses
</commit_message>
<xml_diff>
--- a/documentation/Planning.xlsx
+++ b/documentation/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsaccone\Desktop\ProjectVSCode\tpi-luca\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762597A6-005C-4AA2-8FDF-166BA79C0D9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50907BC-C666-411C-B303-CF1B119AF77B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{168C311F-2955-42E9-B4B5-6A0BF748DD66}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
   <si>
     <t>Vision du planning</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>Documentation de l'API(user manual)</t>
+  </si>
+  <si>
+    <t>Ecriture route GET getDevicesWithAllParameters avec sa requete SQL</t>
+  </si>
+  <si>
+    <t>Ecriture route GET  getDevices avec sa requete SQL</t>
+  </si>
+  <si>
+    <t>Ecriture route POST PostADevice avec sa requete SQL</t>
+  </si>
+  <si>
+    <t>Test Unitaire</t>
+  </si>
+  <si>
+    <t>Ecriture route DELETE deleteDevice avec sa requete SQL</t>
   </si>
 </sst>
 </file>
@@ -471,15 +486,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F184423-44B6-4305-9882-1EF16B7369ED}">
-  <dimension ref="A2:AW36"/>
+  <dimension ref="A2:AW37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
@@ -1088,47 +1103,69 @@
         <v>22</v>
       </c>
       <c r="M28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="U28" s="1"/>
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="T31" s="1"/>
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="J36" s="1"/>
+      <c r="J37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="24">

</xml_diff>

<commit_message>
Documentation of the code
</commit_message>
<xml_diff>
--- a/documentation/Planning.xlsx
+++ b/documentation/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsaccone\Desktop\ProjectVSCode\tpi-luca\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4CA814-7CC1-4844-8B48-3E952A2E0B06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CB2A6B-A5E2-461A-A77B-B6A53B65C210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{168C311F-2955-42E9-B4B5-6A0BF748DD66}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="33">
   <si>
     <t>Vision du planning</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Documentation du code + documentation (word)</t>
+  </si>
+  <si>
+    <t>Implementation de login/ creation de sa route avec sa requete SQL</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A2:AW39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,6 +1120,7 @@
       <c r="U28" s="1"/>
       <c r="AI28" s="1"/>
       <c r="AK28" s="1"/>
+      <c r="AN28" s="1"/>
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1144,7 +1148,7 @@
       </c>
       <c r="U32" s="1"/>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1161,8 +1165,10 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
       <c r="AJ33" s="1"/>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AN33" s="1"/>
+      <c r="AO33" s="1"/>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1170,28 +1176,30 @@
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1199,18 +1207,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AT20:AW20"/>
-    <mergeCell ref="V20:Y20"/>
-    <mergeCell ref="Z20:AC20"/>
-    <mergeCell ref="AD20:AG20"/>
-    <mergeCell ref="AH20:AK20"/>
-    <mergeCell ref="AL20:AO20"/>
-    <mergeCell ref="AP20:AS20"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="R20:U20"/>
     <mergeCell ref="AT2:AW2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:U2"/>
@@ -1223,6 +1219,18 @@
     <mergeCell ref="AH2:AK2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="R20:U20"/>
+    <mergeCell ref="AT20:AW20"/>
+    <mergeCell ref="V20:Y20"/>
+    <mergeCell ref="Z20:AC20"/>
+    <mergeCell ref="AD20:AG20"/>
+    <mergeCell ref="AH20:AK20"/>
+    <mergeCell ref="AL20:AO20"/>
+    <mergeCell ref="AP20:AS20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>